<commit_message>
korea edit page 2021-07-20 17:35:13
</commit_message>
<xml_diff>
--- a/src/views/admin/students/studentsFile.xlsx
+++ b/src/views/admin/students/studentsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/careershe03/Desktop/front-korea/admin/src/views/admin/students/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BFD6891-4530-F442-8C19-056E855EF478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F51EE6-88E4-E445-A0BC-DA2BA2A3EA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="5500" windowWidth="27260" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5660" yWindow="5460" windowWidth="27260" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="学生信息导入模板" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>学号（必填）</t>
   </si>
@@ -85,6 +85,21 @@
   <si>
     <t>高一1班</t>
   </si>
+  <si>
+    <t>999</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>高二</t>
+  </si>
+  <si>
+    <t>高二2班</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +138,14 @@
     <font>
       <sz val="9"/>
       <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -170,7 +193,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -196,6 +219,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -478,11 +504,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -537,6 +563,26 @@
       </c>
       <c r="F2" s="7" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2021</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>